<commit_message>
Fonctionne pour kmeans sans images affichees de chaque cluster
</commit_message>
<xml_diff>
--- a/src/donnees/save_metric.xlsx
+++ b/src/donnees/save_metric.xlsx
@@ -482,25 +482,25 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0</v>
+        <v>0.02945876155425095</v>
       </c>
       <c r="B2" t="n">
-        <v>0</v>
+        <v>0.01311037153586959</v>
       </c>
       <c r="C2" t="n">
-        <v>0.0799725204706192</v>
+        <v>0.06656293570995331</v>
       </c>
       <c r="D2" t="n">
-        <v>1</v>
+        <v>0.09571917679092891</v>
       </c>
       <c r="E2" t="n">
-        <v>0</v>
+        <v>0.1010650535901036</v>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>0.09831950165157408</v>
       </c>
       <c r="G2" t="n">
-        <v>0.003571428571428571</v>
+        <v>0.02212682503993733</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
@@ -515,25 +515,25 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>0</v>
+        <v>0.0256605539773967</v>
       </c>
       <c r="B3" t="n">
-        <v>0</v>
+        <v>0.006366920114159035</v>
       </c>
       <c r="C3" t="n">
-        <v>0.002944193751862349</v>
+        <v>-0.0001098602136784834</v>
       </c>
       <c r="D3" t="n">
-        <v>1</v>
+        <v>0.06714538635729685</v>
       </c>
       <c r="E3" t="n">
-        <v>0</v>
+        <v>0.1071017884686087</v>
       </c>
       <c r="F3" t="n">
-        <v>0</v>
+        <v>0.08254241107171234</v>
       </c>
       <c r="G3" t="n">
-        <v>0.01544117647058824</v>
+        <v>0.01421324605583855</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
@@ -548,25 +548,25 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>0</v>
+        <v>0.05293339361165284</v>
       </c>
       <c r="B4" t="n">
-        <v>0</v>
+        <v>0.02376518639059167</v>
       </c>
       <c r="C4" t="n">
-        <v>0.07287894934415817</v>
+        <v>0.08916099369525909</v>
       </c>
       <c r="D4" t="n">
-        <v>1</v>
+        <v>0.1199266885533998</v>
       </c>
       <c r="E4" t="n">
-        <v>0</v>
+        <v>0.1229736461815776</v>
       </c>
       <c r="F4" t="n">
-        <v>0</v>
+        <v>0.1214310567499631</v>
       </c>
       <c r="G4" t="n">
-        <v>0.01838235294117647</v>
+        <v>0.01884775292497626</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
@@ -581,25 +581,25 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>0</v>
+        <v>0.009527505046701629</v>
       </c>
       <c r="B5" t="n">
-        <v>0</v>
+        <v>0.004116908519828647</v>
       </c>
       <c r="C5" t="n">
-        <v>0.005838770278076849</v>
+        <v>0.00212103851009383</v>
       </c>
       <c r="D5" t="n">
-        <v>1</v>
+        <v>0.07533879614787674</v>
       </c>
       <c r="E5" t="n">
-        <v>0</v>
+        <v>0.08440496493810191</v>
       </c>
       <c r="F5" t="n">
-        <v>0</v>
+        <v>0.0796146078458459</v>
       </c>
       <c r="G5" t="n">
-        <v>0.01081932773109244</v>
+        <v>0.0147208954938141</v>
       </c>
       <c r="H5" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Fonctionne pour kmeans AVEC images affichees de chaque cluster
</commit_message>
<xml_diff>
--- a/src/donnees/save_metric.xlsx
+++ b/src/donnees/save_metric.xlsx
@@ -482,25 +482,25 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0.02945876155425095</v>
+        <v>0.0248213576677426</v>
       </c>
       <c r="B2" t="n">
-        <v>0.01311037153586959</v>
+        <v>0.009190559660654225</v>
       </c>
       <c r="C2" t="n">
-        <v>0.06656293570995331</v>
+        <v>0.07193214446306229</v>
       </c>
       <c r="D2" t="n">
-        <v>0.09571917679092891</v>
+        <v>0.09174852557694076</v>
       </c>
       <c r="E2" t="n">
-        <v>0.1010650535901036</v>
+        <v>0.09499251063071806</v>
       </c>
       <c r="F2" t="n">
-        <v>0.09831950165157408</v>
+        <v>0.09334234154648872</v>
       </c>
       <c r="G2" t="n">
-        <v>0.02212682503993733</v>
+        <v>0.0260220912641523</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
@@ -515,25 +515,25 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>0.0256605539773967</v>
+        <v>0.02554079966903386</v>
       </c>
       <c r="B3" t="n">
-        <v>0.006366920114159035</v>
+        <v>0.004648160779900539</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.0001098602136784834</v>
+        <v>-0.005592891294911867</v>
       </c>
       <c r="D3" t="n">
-        <v>0.06714538635729685</v>
+        <v>0.05676937660284444</v>
       </c>
       <c r="E3" t="n">
-        <v>0.1071017884686087</v>
+        <v>0.1065174908767818</v>
       </c>
       <c r="F3" t="n">
-        <v>0.08254241107171234</v>
+        <v>0.07406513025462461</v>
       </c>
       <c r="G3" t="n">
-        <v>0.01421324605583855</v>
+        <v>0.01197793127816921</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
@@ -548,25 +548,25 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>0.05293339361165284</v>
+        <v>0.06581173914934509</v>
       </c>
       <c r="B4" t="n">
-        <v>0.02376518639059167</v>
+        <v>0.02931022851194365</v>
       </c>
       <c r="C4" t="n">
-        <v>0.08916099369525909</v>
+        <v>0.08717288821935654</v>
       </c>
       <c r="D4" t="n">
-        <v>0.1199266885533998</v>
+        <v>0.1316837502792451</v>
       </c>
       <c r="E4" t="n">
-        <v>0.1229736461815776</v>
+        <v>0.1344966250960489</v>
       </c>
       <c r="F4" t="n">
-        <v>0.1214310567499631</v>
+        <v>0.1330753250879459</v>
       </c>
       <c r="G4" t="n">
-        <v>0.01884775292497626</v>
+        <v>0.02842338630346995</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
@@ -581,25 +581,25 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>0.009527505046701629</v>
+        <v>-0.003432642124829049</v>
       </c>
       <c r="B5" t="n">
-        <v>0.004116908519828647</v>
+        <v>-0.0006012367432928545</v>
       </c>
       <c r="C5" t="n">
-        <v>0.00212103851009383</v>
+        <v>0.001902705547299353</v>
       </c>
       <c r="D5" t="n">
-        <v>0.07533879614787674</v>
+        <v>0.06803268640457041</v>
       </c>
       <c r="E5" t="n">
-        <v>0.08440496493810191</v>
+        <v>0.07284204907249862</v>
       </c>
       <c r="F5" t="n">
-        <v>0.0796146078458459</v>
+        <v>0.07035527363843443</v>
       </c>
       <c r="G5" t="n">
-        <v>0.0147208954938141</v>
+        <v>0.02251122182635113</v>
       </c>
       <c r="H5" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Ajout du modele kmoids
</commit_message>
<xml_diff>
--- a/src/donnees/save_metric.xlsx
+++ b/src/donnees/save_metric.xlsx
@@ -482,25 +482,25 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0.0248213576677426</v>
+        <v>0.02732947460379011</v>
       </c>
       <c r="B2" t="n">
-        <v>0.009190559660654225</v>
+        <v>0.008099341481096272</v>
       </c>
       <c r="C2" t="n">
-        <v>0.07193214446306229</v>
+        <v>0.04823371022939682</v>
       </c>
       <c r="D2" t="n">
-        <v>0.09174852557694076</v>
+        <v>0.08814053599658071</v>
       </c>
       <c r="E2" t="n">
-        <v>0.09499251063071806</v>
+        <v>0.1009959044756205</v>
       </c>
       <c r="F2" t="n">
-        <v>0.09334234154648872</v>
+        <v>0.09413133853757837</v>
       </c>
       <c r="G2" t="n">
-        <v>0.0260220912641523</v>
+        <v>0.02603567827558224</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
@@ -515,25 +515,25 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>0.02554079966903386</v>
+        <v>0.02100294696079608</v>
       </c>
       <c r="B3" t="n">
-        <v>0.004648160779900539</v>
+        <v>0.006438110103244445</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.005592891294911867</v>
+        <v>-0.01669603289021728</v>
       </c>
       <c r="D3" t="n">
-        <v>0.05676937660284444</v>
+        <v>0.05868442345439766</v>
       </c>
       <c r="E3" t="n">
-        <v>0.1065174908767818</v>
+        <v>0.09840140495944422</v>
       </c>
       <c r="F3" t="n">
-        <v>0.07406513025462461</v>
+        <v>0.07352196917387679</v>
       </c>
       <c r="G3" t="n">
-        <v>0.01197793127816921</v>
+        <v>0.01758599876289391</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
@@ -548,25 +548,25 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>0.06581173914934509</v>
+        <v>0.05426793787707845</v>
       </c>
       <c r="B4" t="n">
-        <v>0.02931022851194365</v>
+        <v>0.02507370232752118</v>
       </c>
       <c r="C4" t="n">
-        <v>0.08717288821935654</v>
+        <v>0.06021424010396004</v>
       </c>
       <c r="D4" t="n">
-        <v>0.1316837502792451</v>
+        <v>0.1191507621515193</v>
       </c>
       <c r="E4" t="n">
-        <v>0.1344966250960489</v>
+        <v>0.1266817804555617</v>
       </c>
       <c r="F4" t="n">
-        <v>0.1330753250879459</v>
+        <v>0.1228009158748118</v>
       </c>
       <c r="G4" t="n">
-        <v>0.02842338630346995</v>
+        <v>0.02242512085877799</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
@@ -581,25 +581,25 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>-0.003432642124829049</v>
+        <v>0.01324707873219017</v>
       </c>
       <c r="B5" t="n">
-        <v>-0.0006012367432928545</v>
+        <v>0.004479855794709306</v>
       </c>
       <c r="C5" t="n">
-        <v>0.001902705547299353</v>
+        <v>-0.0004699623746217008</v>
       </c>
       <c r="D5" t="n">
-        <v>0.06803268640457041</v>
+        <v>0.07868029157330532</v>
       </c>
       <c r="E5" t="n">
-        <v>0.07284204907249862</v>
+        <v>0.09626063126655131</v>
       </c>
       <c r="F5" t="n">
-        <v>0.07035527363843443</v>
+        <v>0.0865871108044384</v>
       </c>
       <c r="G5" t="n">
-        <v>0.02251122182635113</v>
+        <v>0.01819391779573026</v>
       </c>
       <c r="H5" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
ajout CNN : pas oublier changer env 3.11
</commit_message>
<xml_diff>
--- a/src/donnees/save_metric.xlsx
+++ b/src/donnees/save_metric.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -482,25 +482,25 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0.02732947460379011</v>
+        <v>0.03072753924798493</v>
       </c>
       <c r="B2" t="n">
-        <v>0.008099341481096272</v>
+        <v>0.007846346145009038</v>
       </c>
       <c r="C2" t="n">
-        <v>0.04823371022939682</v>
+        <v>0.06582808494567871</v>
       </c>
       <c r="D2" t="n">
-        <v>0.08814053599658071</v>
+        <v>0.09126154182117911</v>
       </c>
       <c r="E2" t="n">
-        <v>0.1009959044756205</v>
+        <v>0.1066511746974878</v>
       </c>
       <c r="F2" t="n">
-        <v>0.09413133853757837</v>
+        <v>0.09835801166434541</v>
       </c>
       <c r="G2" t="n">
-        <v>0.02603567827558224</v>
+        <v>0.02333569645984184</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
@@ -515,25 +515,25 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>0.02100294696079608</v>
+        <v>0.01489915666857287</v>
       </c>
       <c r="B3" t="n">
-        <v>0.006438110103244445</v>
+        <v>0.003310804408225765</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.01669603289021728</v>
+        <v>-0.00726838962117827</v>
       </c>
       <c r="D3" t="n">
-        <v>0.05868442345439766</v>
+        <v>0.04882070088206886</v>
       </c>
       <c r="E3" t="n">
-        <v>0.09840140495944422</v>
+        <v>0.1011448360198526</v>
       </c>
       <c r="F3" t="n">
-        <v>0.07352196917387679</v>
+        <v>0.06585462082959219</v>
       </c>
       <c r="G3" t="n">
-        <v>0.01758599876289391</v>
+        <v>0.01015087145969499</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
@@ -548,25 +548,25 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>0.05426793787707845</v>
+        <v>0.05485779992694893</v>
       </c>
       <c r="B4" t="n">
-        <v>0.02507370232752118</v>
+        <v>0.01750636503375207</v>
       </c>
       <c r="C4" t="n">
-        <v>0.06021424010396004</v>
+        <v>0.07172764837741852</v>
       </c>
       <c r="D4" t="n">
-        <v>0.1191507621515193</v>
+        <v>0.1178446918715434</v>
       </c>
       <c r="E4" t="n">
-        <v>0.1266817804555617</v>
+        <v>0.1258494983977992</v>
       </c>
       <c r="F4" t="n">
-        <v>0.1228009158748118</v>
+        <v>0.121715625181588</v>
       </c>
       <c r="G4" t="n">
-        <v>0.02242512085877799</v>
+        <v>0.02610132981227498</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
@@ -581,25 +581,25 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>0.01324707873219017</v>
+        <v>0.004053295892611886</v>
       </c>
       <c r="B5" t="n">
-        <v>0.004479855794709306</v>
+        <v>0.0007101097404372962</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.0004699623746217008</v>
+        <v>0.004137439861266331</v>
       </c>
       <c r="D5" t="n">
-        <v>0.07868029157330532</v>
+        <v>0.0748104645746592</v>
       </c>
       <c r="E5" t="n">
-        <v>0.09626063126655131</v>
+        <v>0.1010751379315278</v>
       </c>
       <c r="F5" t="n">
-        <v>0.0865871108044384</v>
+        <v>0.08598177358308073</v>
       </c>
       <c r="G5" t="n">
-        <v>0.01819391779573026</v>
+        <v>0.01371640142198511</v>
       </c>
       <c r="H5" t="inlineStr">
         <is>
@@ -607,6 +607,39 @@
         </is>
       </c>
       <c r="I5" t="inlineStr">
+        <is>
+          <t>kmeans</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>0.1342448192655817</v>
+      </c>
+      <c r="B6" t="n">
+        <v>0.0261367725086431</v>
+      </c>
+      <c r="C6" t="n">
+        <v>-0.0216719675809145</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.1605071901277799</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.2475178865761927</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.1947350922724521</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0.01953489584559281</v>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>CNN</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
         <is>
           <t>kmeans</t>
         </is>

</xml_diff>

<commit_message>
Ajout R50 + correction affichage images
</commit_message>
<xml_diff>
--- a/src/donnees/save_metric.xlsx
+++ b/src/donnees/save_metric.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -482,29 +482,29 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0.03072753924798493</v>
+        <v>0.02981232170111252</v>
       </c>
       <c r="B2" t="n">
-        <v>0.007846346145009038</v>
+        <v>0.01030980947691171</v>
       </c>
       <c r="C2" t="n">
-        <v>0.06582808494567871</v>
+        <v>0.07886553555727005</v>
       </c>
       <c r="D2" t="n">
-        <v>0.09126154182117911</v>
+        <v>0.09581993626485329</v>
       </c>
       <c r="E2" t="n">
-        <v>0.1066511746974878</v>
+        <v>0.1019920290467978</v>
       </c>
       <c r="F2" t="n">
-        <v>0.09835801166434541</v>
+        <v>0.09880969240045873</v>
       </c>
       <c r="G2" t="n">
-        <v>0.02333569645984184</v>
+        <v>0.0264176699616247</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>HISTOGRAM</t>
+          <t>HIST</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
@@ -515,25 +515,25 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>0.01489915666857287</v>
+        <v>0.02790758206592524</v>
       </c>
       <c r="B3" t="n">
-        <v>0.003310804408225765</v>
+        <v>0.006167315309216211</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.00726838962117827</v>
+        <v>0.002642247483078762</v>
       </c>
       <c r="D3" t="n">
-        <v>0.04882070088206886</v>
+        <v>0.07064315185672221</v>
       </c>
       <c r="E3" t="n">
-        <v>0.1011448360198526</v>
+        <v>0.1154623178720089</v>
       </c>
       <c r="F3" t="n">
-        <v>0.06585462082959219</v>
+        <v>0.08765590895367681</v>
       </c>
       <c r="G3" t="n">
-        <v>0.01015087145969499</v>
+        <v>0.01481525358142623</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
@@ -548,25 +548,25 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>0.05485779992694893</v>
+        <v>0.0578885796578331</v>
       </c>
       <c r="B4" t="n">
-        <v>0.01750636503375207</v>
+        <v>0.02143430655904847</v>
       </c>
       <c r="C4" t="n">
-        <v>0.07172764837741852</v>
+        <v>0.07993114739656448</v>
       </c>
       <c r="D4" t="n">
-        <v>0.1178446918715434</v>
+        <v>0.1241097434545708</v>
       </c>
       <c r="E4" t="n">
-        <v>0.1258494983977992</v>
+        <v>0.1286966308993251</v>
       </c>
       <c r="F4" t="n">
-        <v>0.121715625181588</v>
+        <v>0.1263615752190126</v>
       </c>
       <c r="G4" t="n">
-        <v>0.02610132981227498</v>
+        <v>0.02338304711220633</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
@@ -581,25 +581,25 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>0.004053295892611886</v>
+        <v>0.00258757531719792</v>
       </c>
       <c r="B5" t="n">
-        <v>0.0007101097404372962</v>
+        <v>0.0008886521614781591</v>
       </c>
       <c r="C5" t="n">
-        <v>0.004137439861266331</v>
+        <v>0.0002865124396746043</v>
       </c>
       <c r="D5" t="n">
-        <v>0.0748104645746592</v>
+        <v>0.07399011370985233</v>
       </c>
       <c r="E5" t="n">
-        <v>0.1010751379315278</v>
+        <v>0.0781784438921367</v>
       </c>
       <c r="F5" t="n">
-        <v>0.08598177358308073</v>
+        <v>0.07602663841196711</v>
       </c>
       <c r="G5" t="n">
-        <v>0.01371640142198511</v>
+        <v>0.0241775575112623</v>
       </c>
       <c r="H5" t="inlineStr">
         <is>
@@ -614,25 +614,25 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>0.1342448192655817</v>
+        <v>0.1868782761963731</v>
       </c>
       <c r="B6" t="n">
-        <v>0.0261367725086431</v>
+        <v>0.07645071511630383</v>
       </c>
       <c r="C6" t="n">
-        <v>-0.0216719675809145</v>
+        <v>0.004124026745557785</v>
       </c>
       <c r="D6" t="n">
-        <v>0.1605071901277799</v>
+        <v>0.2248082921625947</v>
       </c>
       <c r="E6" t="n">
-        <v>0.2475178865761927</v>
+        <v>0.261170731249527</v>
       </c>
       <c r="F6" t="n">
-        <v>0.1947350922724521</v>
+        <v>0.2416291371706875</v>
       </c>
       <c r="G6" t="n">
-        <v>0.01953489584559281</v>
+        <v>0.01727697423717817</v>
       </c>
       <c r="H6" t="inlineStr">
         <is>
@@ -640,6 +640,39 @@
         </is>
       </c>
       <c r="I6" t="inlineStr">
+        <is>
+          <t>kmeans</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>0.2749036812750683</v>
+      </c>
+      <c r="B7" t="n">
+        <v>0.1212951601526189</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.02451329305768013</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.3094482230614211</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.3451583395644867</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.3263292516488247</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0.01308993932176823</v>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>RESNET</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
         <is>
           <t>kmeans</t>
         </is>

</xml_diff>